<commit_message>
Optimized Leave Application Test Cases
</commit_message>
<xml_diff>
--- a/testData/timetracker_bryan.xlsx
+++ b/testData/timetracker_bryan.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -44,225 +44,7 @@
     <t xml:space="preserve">accountWithZeroVacationLeaveBalance</t>
   </si>
   <si>
-    <t xml:space="preserve">leaveTypes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">testComment</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF2A00FF"/>
-        <rFont val="JetBrains Mono ExtraLight"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">"Bank General Leave"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <rFont val="JetBrains Mono ExtraLight"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF2A00FF"/>
-        <rFont val="JetBrains Mono ExtraLight"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">"Call Back Vacation Leave"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <rFont val="JetBrains Mono ExtraLight"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF2A00FF"/>
-        <rFont val="JetBrains Mono ExtraLight"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">"Excess Earned Leaves"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <rFont val="JetBrains Mono ExtraLight"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF2A00FF"/>
-        <rFont val="JetBrains Mono ExtraLight"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">"Excess General Leaves"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <rFont val="JetBrains Mono ExtraLight"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF2A00FF"/>
-        <rFont val="JetBrains Mono ExtraLight"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">"General Leave"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <rFont val="JetBrains Mono ExtraLight"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF2A00FF"/>
-        <rFont val="JetBrains Mono ExtraLight"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">"Leave Without Pay"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <rFont val="JetBrains Mono ExtraLight"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF2A00FF"/>
-        <rFont val="JetBrains Mono ExtraLight"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">"On-call Vacation Leave"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <rFont val="JetBrains Mono ExtraLight"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF2A00FF"/>
-        <rFont val="JetBrains Mono ExtraLight"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">"Overtime Vacation Leave"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <rFont val="JetBrains Mono ExtraLight"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF2A00FF"/>
-        <rFont val="JetBrains Mono ExtraLight"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">"Service Incentive Leave"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <rFont val="JetBrains Mono ExtraLight"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF2A00FF"/>
-        <rFont val="JetBrains Mono ExtraLight"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">"Solo Parent Leave"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <rFont val="JetBrains Mono ExtraLight"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF2A00FF"/>
-        <rFont val="JetBrains Mono ExtraLight"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">"Unauthorized LWOP"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <rFont val="JetBrains Mono ExtraLight"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF2A00FF"/>
-        <rFont val="JetBrains Mono ExtraLight"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">"Vacation Leave"</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">TC008</t>
-  </si>
-  <si>
-    <t xml:space="preserve">“TEST COMMENT/REMARK”</t>
+    <t xml:space="preserve">expectedFromAndToDateFormat</t>
   </si>
 </sst>
 </file>
@@ -272,7 +54,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -306,6 +88,7 @@
       <color rgb="FF000000"/>
       <name val="JetBrains Mono ExtraLight"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -313,12 +96,19 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF0000C0"/>
+      <name val="JetBrains Mono ExtraLight"/>
+      <family val="0"/>
     </font>
     <font>
       <sz val="9"/>
       <color rgb="FF2A00FF"/>
       <name val="JetBrains Mono ExtraLight"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -363,7 +153,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -385,6 +175,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -403,7 +197,7 @@
       <rgbColor rgb="FFFFFFFF"/>
       <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF2A00FF"/>
+      <rgbColor rgb="FF0000C0"/>
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
@@ -430,7 +224,7 @@
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF800000"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF2A00FF"/>
       <rgbColor rgb="FF00CCFF"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FFCCFFCC"/>
@@ -468,7 +262,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -528,10 +322,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
+      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -545,28 +339,13 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>11</v>
-      </c>
+      <c r="C1" s="1"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="6"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>